<commit_message>
data logging improved + some other things
</commit_message>
<xml_diff>
--- a/Glow/ExampleCsv.xlsx
+++ b/Glow/ExampleCsv.xlsx
@@ -58,9 +58,6 @@
     <t>direction foot/hand should point (1 = forward, 2 = right, 3 = backwards, 4 = left)</t>
   </si>
   <si>
-    <t>time (seconds) at which to pause video for pressure sensing feedback</t>
-  </si>
-  <si>
     <t>Area 1</t>
   </si>
   <si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>Area 4</t>
+  </si>
+  <si>
+    <t>time (seconds) at which to: pause video for pressure sensing feedback, transition into pose, and transition out of pose</t>
   </si>
 </sst>
 </file>
@@ -963,7 +963,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,16 +1755,16 @@
         <v>40</v>
       </c>
       <c r="B30" s="2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -1780,16 +1780,16 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>